<commit_message>
updates to Max Abund for DNR
</commit_message>
<xml_diff>
--- a/Max_Abund_Final_Pasture_DNR.xlsx
+++ b/Max_Abund_Final_Pasture_DNR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rozzer/Library/CloudStorage/Dropbox/_Manuscripts/BirdCommCode/Bird-Comm-Code-All/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{351ED999-EB5F-424D-861E-40F0292079DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{2ABBB81D-99E1-574B-B383-A01004445937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35400" yWindow="-10660" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="620" yWindow="760" windowWidth="28040" windowHeight="17440"/>
   </bookViews>
   <sheets>
     <sheet name="Max_Abund_Final_Pasture_DNR" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>year</t>
   </si>
@@ -88,9 +88,6 @@
     <t>SEWR</t>
   </si>
   <si>
-    <t>GRPC</t>
-  </si>
-  <si>
     <t>VESP</t>
   </si>
   <si>
@@ -137,15 +134,6 @@
   </si>
   <si>
     <t>KILL</t>
-  </si>
-  <si>
-    <t>HOLA</t>
-  </si>
-  <si>
-    <t>TUVU</t>
-  </si>
-  <si>
-    <t>AMKE</t>
   </si>
   <si>
     <t>BEVI</t>
@@ -1010,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:O11"/>
+      <selection activeCell="P21" sqref="D11:P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1388,7 +1376,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8">
         <v>2023</v>
@@ -1403,7 +1391,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1418,7 +1406,7 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1427,7 +1415,7 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="O8">
         <v>0</v>
@@ -1441,7 +1429,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>2023</v>
@@ -1456,7 +1444,7 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0.06</v>
+        <v>0.18</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1471,7 +1459,7 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1480,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="N9">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="O9">
         <v>0</v>
@@ -1494,7 +1482,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>2023</v>
@@ -1503,13 +1491,13 @@
         <v>24</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0.18</v>
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1518,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1542,118 +1530,118 @@
         <v>0</v>
       </c>
       <c r="Q10" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>2023</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D11">
-        <v>0.28000000000000003</v>
+        <v>0.93</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.47</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="I11">
-        <v>0.12</v>
+        <v>0.92</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>0.62</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>0.47</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>1.03</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>0.33</v>
       </c>
       <c r="P11">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="Q11" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>2023</v>
       </c>
       <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12">
+        <v>0.74</v>
+      </c>
+      <c r="E12">
+        <v>1.5</v>
+      </c>
+      <c r="F12">
+        <v>0.65</v>
+      </c>
+      <c r="G12">
+        <v>0.33</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0.6</v>
+      </c>
+      <c r="J12">
+        <v>0.12</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0.83</v>
+      </c>
+      <c r="M12">
+        <v>2.06</v>
+      </c>
+      <c r="N12">
+        <v>0.17</v>
+      </c>
+      <c r="O12">
+        <v>1.42</v>
+      </c>
+      <c r="P12">
+        <v>0.67</v>
+      </c>
+      <c r="Q12" t="s">
         <v>27</v>
-      </c>
-      <c r="D12">
-        <v>0.93</v>
-      </c>
-      <c r="E12">
-        <v>0.3</v>
-      </c>
-      <c r="F12">
-        <v>0.47</v>
-      </c>
-      <c r="G12">
-        <v>0.11</v>
-      </c>
-      <c r="H12">
-        <v>0.4</v>
-      </c>
-      <c r="I12">
-        <v>0.92</v>
-      </c>
-      <c r="J12">
-        <v>0.62</v>
-      </c>
-      <c r="K12">
-        <v>0.47</v>
-      </c>
-      <c r="L12">
-        <v>0.33</v>
-      </c>
-      <c r="M12">
-        <v>1.03</v>
-      </c>
-      <c r="N12">
-        <v>0.5</v>
-      </c>
-      <c r="O12">
-        <v>0.33</v>
-      </c>
-      <c r="P12">
-        <v>0.4</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>2023</v>
@@ -1662,51 +1650,51 @@
         <v>29</v>
       </c>
       <c r="D13">
-        <v>0.74</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>1.5</v>
+        <v>0.1</v>
       </c>
       <c r="F13">
-        <v>0.65</v>
+        <v>0.06</v>
       </c>
       <c r="G13">
-        <v>0.33</v>
+        <v>0.11</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0.6</v>
+        <v>0.04</v>
       </c>
       <c r="J13">
         <v>0.12</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>0.31</v>
       </c>
       <c r="L13">
-        <v>0.83</v>
+        <v>1</v>
       </c>
       <c r="M13">
-        <v>2.06</v>
+        <v>0.52</v>
       </c>
       <c r="N13">
-        <v>0.17</v>
+        <v>0.67</v>
       </c>
       <c r="O13">
-        <v>1.42</v>
+        <v>0.25</v>
       </c>
       <c r="P13">
-        <v>0.67</v>
+        <v>0.53</v>
       </c>
       <c r="Q13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <v>2023</v>
@@ -1721,45 +1709,45 @@
         <v>0.1</v>
       </c>
       <c r="F14">
-        <v>0.06</v>
+        <v>0.71</v>
       </c>
       <c r="G14">
-        <v>0.11</v>
+        <v>0.22</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="I14">
-        <v>0.04</v>
+        <v>0.2</v>
       </c>
       <c r="J14">
-        <v>0.12</v>
+        <v>1.38</v>
       </c>
       <c r="K14">
-        <v>0.31</v>
+        <v>1.25</v>
       </c>
       <c r="L14">
+        <v>0.33</v>
+      </c>
+      <c r="M14">
+        <v>1.29</v>
+      </c>
+      <c r="N14">
         <v>1</v>
       </c>
-      <c r="M14">
-        <v>0.52</v>
-      </c>
-      <c r="N14">
-        <v>0.67</v>
-      </c>
       <c r="O14">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="P14">
-        <v>0.53</v>
+        <v>1.33</v>
       </c>
       <c r="Q14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <v>2023</v>
@@ -1771,48 +1759,48 @@
         <v>0</v>
       </c>
       <c r="E15">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F15">
-        <v>0.71</v>
+        <v>0</v>
       </c>
       <c r="G15">
-        <v>0.22</v>
+        <v>0.11</v>
       </c>
       <c r="H15">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="I15">
-        <v>0.2</v>
+        <v>0.04</v>
       </c>
       <c r="J15">
-        <v>1.38</v>
+        <v>0</v>
       </c>
       <c r="K15">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>1.29</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O15">
         <v>0</v>
       </c>
       <c r="P15">
-        <v>1.33</v>
+        <v>0</v>
       </c>
       <c r="Q15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>2023</v>
@@ -1824,48 +1812,48 @@
         <v>0</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="G16">
         <v>0.11</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="I16">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>0.62</v>
       </c>
       <c r="K16">
         <v>0</v>
       </c>
       <c r="L16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="Q16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>2023</v>
@@ -1877,48 +1865,48 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F17">
-        <v>0.28999999999999998</v>
+        <v>0.06</v>
       </c>
       <c r="G17">
-        <v>0.11</v>
+        <v>0</v>
       </c>
       <c r="H17">
-        <v>0.27</v>
+        <v>0.13</v>
       </c>
       <c r="I17">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="J17">
-        <v>0.62</v>
+        <v>0</v>
       </c>
       <c r="K17">
         <v>0</v>
       </c>
       <c r="L17">
-        <v>0.5</v>
+        <v>0.17</v>
       </c>
       <c r="M17">
-        <v>0</v>
+        <v>0.26</v>
       </c>
       <c r="N17">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="O17">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="P17">
-        <v>0.27</v>
+        <v>0</v>
       </c>
       <c r="Q17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <v>2023</v>
@@ -1933,31 +1921,31 @@
         <v>0</v>
       </c>
       <c r="F18">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="G18">
         <v>0</v>
       </c>
       <c r="H18">
-        <v>0.13</v>
+        <v>0</v>
       </c>
       <c r="I18">
-        <v>0.12</v>
+        <v>0.04</v>
       </c>
       <c r="J18">
         <v>0</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="L18">
         <v>0.17</v>
       </c>
       <c r="M18">
-        <v>0.26</v>
+        <v>0.39</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -1966,12 +1954,12 @@
         <v>0</v>
       </c>
       <c r="Q18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>2023</v>
@@ -1980,10 +1968,10 @@
         <v>35</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1995,22 +1983,22 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <v>0</v>
       </c>
       <c r="K19">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="L19">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="M19">
-        <v>0.39</v>
+        <v>0</v>
       </c>
       <c r="N19">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="O19">
         <v>0</v>
@@ -2019,12 +2007,12 @@
         <v>0</v>
       </c>
       <c r="Q19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>2023</v>
@@ -2033,13 +2021,13 @@
         <v>36</v>
       </c>
       <c r="D20">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="E20">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>0.41</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -2054,7 +2042,7 @@
         <v>0</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -2072,12 +2060,12 @@
         <v>0</v>
       </c>
       <c r="Q20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>2023</v>
@@ -2089,10 +2077,10 @@
         <v>0</v>
       </c>
       <c r="E21">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>0.41</v>
+        <v>0.06</v>
       </c>
       <c r="G21">
         <v>0</v>
@@ -2101,13 +2089,13 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="J21">
         <v>0</v>
       </c>
       <c r="K21">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -2125,12 +2113,12 @@
         <v>0</v>
       </c>
       <c r="Q21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B22">
         <v>2023</v>
@@ -2142,10 +2130,10 @@
         <v>0</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F22">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -2154,16 +2142,16 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <v>0</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -2175,157 +2163,157 @@
         <v>0</v>
       </c>
       <c r="P22">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="Q22" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B23">
         <v>2023</v>
       </c>
       <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0.04</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0.13</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0.08</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="s">
         <v>39</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>0</v>
-      </c>
-      <c r="I23">
-        <v>0</v>
-      </c>
-      <c r="J23">
-        <v>0</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-      <c r="M23">
-        <v>0</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>2023</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>0.18</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
       <c r="I24">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>0.86</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="N24">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="O24">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="P24">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="Q24" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>2023</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
       <c r="H25">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="I25">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J25">
         <v>0</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
       <c r="M25">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -2337,65 +2325,65 @@
         <v>0</v>
       </c>
       <c r="Q25" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B26">
         <v>2023</v>
       </c>
       <c r="C26" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="G26">
         <v>0</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K26">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0.13</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
         <v>0.17</v>
-      </c>
-      <c r="M26">
-        <v>0</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26">
-        <v>0</v>
       </c>
       <c r="P26">
         <v>0.13</v>
       </c>
       <c r="Q26" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B27">
         <v>2023</v>
@@ -2407,22 +2395,22 @@
         <v>0</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="G27">
         <v>0</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="I27">
-        <v>0.04</v>
+        <v>0.2</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -2437,18 +2425,18 @@
         <v>0</v>
       </c>
       <c r="O27">
-        <v>0.08</v>
+        <v>0.17</v>
       </c>
       <c r="P27">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="Q27" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B28">
         <v>2023</v>
@@ -2460,258 +2448,95 @@
         <v>0</v>
       </c>
       <c r="E28">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
       <c r="F28">
-        <v>0.18</v>
+        <v>0.24</v>
       </c>
       <c r="G28">
         <v>0.11</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="I28">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="J28">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="K28">
-        <v>0.86</v>
+        <v>0</v>
       </c>
       <c r="L28">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="M28">
-        <v>0.65</v>
+        <v>0</v>
       </c>
       <c r="N28">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="O28">
-        <v>0.08</v>
+        <v>0</v>
       </c>
       <c r="P28">
-        <v>0.67</v>
+        <v>0</v>
       </c>
       <c r="Q28" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>2023</v>
-      </c>
-      <c r="C29" t="s">
-        <v>46</v>
-      </c>
-      <c r="D29">
-        <v>0.09</v>
-      </c>
-      <c r="E29">
-        <v>0.4</v>
-      </c>
-      <c r="F29">
-        <v>0.35</v>
-      </c>
-      <c r="G29">
-        <v>0</v>
-      </c>
-      <c r="H29">
-        <v>0.13</v>
-      </c>
-      <c r="I29">
-        <v>0.2</v>
-      </c>
-      <c r="J29">
-        <v>0</v>
-      </c>
-      <c r="K29">
-        <v>0.16</v>
-      </c>
-      <c r="L29">
-        <v>0</v>
-      </c>
-      <c r="M29">
-        <v>0.13</v>
-      </c>
-      <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="O29">
-        <v>0</v>
-      </c>
-      <c r="P29">
-        <v>0</v>
-      </c>
-      <c r="Q29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>2023</v>
-      </c>
-      <c r="C30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <v>0.2</v>
-      </c>
-      <c r="F30">
-        <v>0.12</v>
-      </c>
-      <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30">
-        <v>0.13</v>
-      </c>
-      <c r="I30">
-        <v>0.2</v>
-      </c>
-      <c r="J30">
-        <v>0.25</v>
-      </c>
-      <c r="K30">
-        <v>0</v>
-      </c>
-      <c r="L30">
-        <v>0</v>
-      </c>
-      <c r="M30">
-        <v>0.13</v>
-      </c>
-      <c r="N30">
-        <v>0</v>
-      </c>
-      <c r="O30">
-        <v>0.17</v>
-      </c>
-      <c r="P30">
-        <v>0.13</v>
-      </c>
-      <c r="Q30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>2023</v>
-      </c>
-      <c r="C31" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31">
-        <v>0</v>
-      </c>
-      <c r="E31">
-        <v>0.2</v>
-      </c>
-      <c r="F31">
-        <v>0.12</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>0.13</v>
-      </c>
-      <c r="I31">
-        <v>0.2</v>
-      </c>
-      <c r="J31">
-        <v>0.25</v>
-      </c>
-      <c r="K31">
-        <v>0</v>
-      </c>
-      <c r="L31">
-        <v>0</v>
-      </c>
-      <c r="M31">
-        <v>0.13</v>
-      </c>
-      <c r="N31">
-        <v>0</v>
-      </c>
-      <c r="O31">
-        <v>0.17</v>
-      </c>
-      <c r="P31">
-        <v>0.13</v>
-      </c>
-      <c r="Q31" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>2023</v>
-      </c>
-      <c r="C32" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0.4</v>
-      </c>
-      <c r="F32">
-        <v>0.24</v>
-      </c>
-      <c r="G32">
-        <v>0.11</v>
-      </c>
-      <c r="H32">
-        <v>0.13</v>
-      </c>
-      <c r="I32">
-        <v>0.08</v>
-      </c>
-      <c r="J32">
-        <v>0</v>
-      </c>
-      <c r="K32">
-        <v>0</v>
-      </c>
-      <c r="L32">
-        <v>0</v>
-      </c>
-      <c r="M32">
-        <v>0</v>
-      </c>
-      <c r="N32">
-        <v>0</v>
-      </c>
-      <c r="O32">
-        <v>0</v>
-      </c>
-      <c r="P32">
-        <v>0</v>
-      </c>
-      <c r="Q32" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D22:P28">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:O10">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P10">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11:P21">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>